<commit_message>
updated defect tracking list with faults fixed
</commit_message>
<xml_diff>
--- a/documentation/defect_tracking.xlsx
+++ b/documentation/defect_tracking.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/landen/Desktop/Classes/Spring22/eecs448/Project4/ds_visualizerProject4/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Z\Desktop\Battleship Game Project 1 EECS448\Project 4\ds_visualizerProject4\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5F2189F-AAFD-C946-AA47-46842008C798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7464EB9B-8B1B-4B61-AC30-578ECB27B519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35160" yWindow="2340" windowWidth="27640" windowHeight="16440" xr2:uid="{27BA6C2D-5EA5-1548-A7AF-B2E08A2B94C7}"/>
+    <workbookView xWindow="1725" yWindow="1680" windowWidth="26520" windowHeight="11385" xr2:uid="{27BA6C2D-5EA5-1548-A7AF-B2E08A2B94C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Date Discovered</t>
   </si>
@@ -53,6 +52,66 @@
   </si>
   <si>
     <t>Description of Fix</t>
+  </si>
+  <si>
+    <t>BST nodes does not appear as expected</t>
+  </si>
+  <si>
+    <t>Switch the browser to run the program</t>
+  </si>
+  <si>
+    <t>Stack function push accepts null as valid inputs</t>
+  </si>
+  <si>
+    <t>Stack function push accepts empty string as valid inputs</t>
+  </si>
+  <si>
+    <t>Added an if statement to catch null and restart the function</t>
+  </si>
+  <si>
+    <t>Added an if statement to catch empty string and restart the function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aidan </t>
+  </si>
+  <si>
+    <t>Duy</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>Landen</t>
+  </si>
+  <si>
+    <t>Queue function enqueue accepts empty strings as valid input</t>
+  </si>
+  <si>
+    <t>Aidan</t>
+  </si>
+  <si>
+    <t>Added if statement to return to main function page after user enters empty string</t>
+  </si>
+  <si>
+    <t>Queue function enqueue accepts cancel input from user</t>
+  </si>
+  <si>
+    <t>Added if statement to catch the cancel input which gives null and returns the user into the main page of queue</t>
+  </si>
+  <si>
+    <t>Linked List insert accepts empty string as a valid input</t>
+  </si>
+  <si>
+    <t>Added another if statement to catch the empty string to return the user back to main page of linked list so they can input again</t>
+  </si>
+  <si>
+    <t>Linked List insert accepts cancel from user as a valid input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eric </t>
+  </si>
+  <si>
+    <t>Added if statement to make sure that cancel is not accepted as a input and returns the user back to the main page of linked list to input a valid input</t>
   </si>
 </sst>
 </file>
@@ -123,10 +182,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,21 +503,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67CB543-2F2C-8A4E-B7E0-E5A18D6B864C}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="124.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -477,22 +537,150 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>44674</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44671</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>44671</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44671</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44671</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3">
+        <v>44672</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>44672</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44672</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="21.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>44672</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44673</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="21.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>44673</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3">
+        <v>44673</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="21.75" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3">
+        <v>44674</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="21.75" x14ac:dyDescent="0.3">
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="21.75" x14ac:dyDescent="0.3">
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="21.75" x14ac:dyDescent="0.3">
       <c r="G11" s="1"/>
     </row>
   </sheetData>

</xml_diff>